<commit_message>
[ADD] TESTE COM LOGIN USANDO DB
</commit_message>
<xml_diff>
--- a/src/credentials/credentials.xlsx
+++ b/src/credentials/credentials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>NOME</t>
   </si>
@@ -28,18 +28,6 @@
     <t>GRUPO_ACESSO</t>
   </si>
   <si>
-    <t>emersona7x@hotmail.com</t>
-  </si>
-  <si>
-    <t>Emerson Rafael</t>
-  </si>
-  <si>
-    <t>$2b$12$uqQZ/j6Bhl7IdTPwLp74s.G/50lijSx6m1EaHZ9gB02R0mitfrOTe</t>
-  </si>
-  <si>
-    <t>ADM</t>
-  </si>
-  <si>
     <t>rbriggs@gmail.com</t>
   </si>
   <si>
@@ -50,9 +38,6 @@
   </si>
   <si>
     <t>EDITORA</t>
-  </si>
-  <si>
-    <t>emervin</t>
   </si>
   <si>
     <t>rbriggs</t>
@@ -403,7 +388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -416,7 +401,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -433,7 +418,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -448,27 +433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>